<commit_message>
Workbooks comparison improved to be version independent. Conditional format formula shifting turned off.
</commit_message>
<xml_diff>
--- a/tests/Gauges/tLists2_sum.xlsx
+++ b/tests/Gauges/tLists2_sum.xlsx
@@ -8,10 +8,11 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="__temp_buffer" sheetId="5" state="veryHidden" r:id="rId5"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Orders">'Sheet1'!$A$12:$J$18</x:definedName>
-    <x:definedName name="Orders_tpl">'Sheet1'!$A$12:$J$13</x:definedName>
+    <x:definedName name="Orders">Sheet1!$A$12:$J$18</x:definedName>
+    <x:definedName name="Orders_tpl">Sheet1!$A$12:$J$13</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
@@ -291,7 +292,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="56">
+  <x:cellStyleXfs count="24">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -305,9 +306,6 @@
     <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -323,39 +321,24 @@
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -368,9 +351,6 @@
     <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -381,81 +361,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="4" fontId="2" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="2" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="8" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -699,7 +604,7 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="3">
+  <x:dxfs count="1">
     <x:dxf>
       <x:font>
         <x:b val="0"/>
@@ -708,24 +613,6 @@
         <x:extend val="0"/>
         <x:color indexed="30"/>
       </x:font>
-    </x:dxf>
-    <x:dxf>
-      <x:font>
-        <x:color indexed="30"/>
-      </x:font>
-      <x:fill>
-        <x:patternFill/>
-      </x:fill>
-      <x:border/>
-    </x:dxf>
-    <x:dxf>
-      <x:font>
-        <x:color indexed="30"/>
-      </x:font>
-      <x:fill>
-        <x:patternFill patternType="solid"/>
-      </x:fill>
-      <x:border/>
     </x:dxf>
   </x:dxfs>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -804,45 +691,38 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>638176</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>629177</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="1895475" cy="609600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2" descr="logo.png"/>
+        <xdr:cNvPr id="1" name="Рисунок 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3295650" y="19050"/>
-          <a:ext cx="1895476" cy="610127"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1895475" cy="609600"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1217,9 +1097,10 @@
     <x:col min="8" max="8" width="9.164062" style="45" customWidth="1"/>
     <x:col min="9" max="9" width="10.832031" style="45" customWidth="1"/>
     <x:col min="10" max="10" width="11.5" style="45" customWidth="1"/>
+    <x:col min="11" max="11" width="9.140625" style="45" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:10" customFormat="1" ht="51" customHeight="1">
+    <x:row r="1" spans="1:11" customFormat="1" ht="51" customHeight="1">
       <x:c r="A1" s="45" t="s"/>
       <x:c r="B1" s="46" t="s">
         <x:v>0</x:v>
@@ -1233,7 +1114,7 @@
       <x:c r="I1" s="47" t="s"/>
       <x:c r="J1" s="47" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:10" customFormat="1" ht="12.75" customHeight="1">
+    <x:row r="2" spans="1:11" customFormat="1" ht="12.75" customHeight="1">
       <x:c r="A2" s="45" t="s"/>
       <x:c r="B2" s="48" t="s"/>
       <x:c r="C2" s="48" t="s"/>
@@ -1245,7 +1126,7 @@
       <x:c r="I2" s="48" t="s"/>
       <x:c r="J2" s="45" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:10" customFormat="1" ht="18" customHeight="1">
+    <x:row r="3" spans="1:11" customFormat="1" ht="18" customHeight="1">
       <x:c r="A3" s="49" t="s"/>
       <x:c r="B3" s="50" t="s">
         <x:v>1</x:v>
@@ -1261,7 +1142,7 @@
       <x:c r="I3" s="53" t="s"/>
       <x:c r="J3" s="54" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:10">
+    <x:row r="4" spans="1:11">
       <x:c r="A4" s="45" t="s"/>
       <x:c r="B4" s="55" t="s"/>
       <x:c r="C4" s="45" t="s"/>
@@ -1273,7 +1154,7 @@
       <x:c r="I4" s="45" t="s"/>
       <x:c r="J4" s="45" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:10">
+    <x:row r="5" spans="1:11">
       <x:c r="A5" s="45" t="s"/>
       <x:c r="B5" s="50" t="s">
         <x:v>3</x:v>
@@ -1286,7 +1167,7 @@
       <x:c r="H5" s="45" t="s"/>
       <x:c r="I5" s="45" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="6" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A6" s="45" t="s"/>
       <x:c r="B6" s="56" t="s">
         <x:f>"4-976 Sugarloaf Hwy"&amp;" "&amp;"Suite 103"</x:f>
@@ -1300,7 +1181,7 @@
       <x:c r="I6" s="59" t="s"/>
       <x:c r="J6" s="60" t="s"/>
     </x:row>
-    <x:row r="7" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="7" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A7" s="45" t="s"/>
       <x:c r="B7" s="61" t="s"/>
       <x:c r="C7" s="62" t="s"/>
@@ -1312,7 +1193,7 @@
       <x:c r="I7" s="45" t="s"/>
       <x:c r="J7" s="45" t="s"/>
     </x:row>
-    <x:row r="8" spans="1:10">
+    <x:row r="8" spans="1:11">
       <x:c r="A8" s="45" t="s"/>
       <x:c r="B8" s="50" t="s">
         <x:v>4</x:v>
@@ -1331,7 +1212,7 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="9" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A9" s="45" t="s"/>
       <x:c r="B9" s="63" t="s">
         <x:v>8</x:v>
@@ -1351,7 +1232,7 @@
       </x:c>
       <x:c r="J9" s="64" t="s"/>
     </x:row>
-    <x:row r="10" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="10" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A10" s="45" t="s"/>
       <x:c r="B10" s="65" t="s"/>
       <x:c r="C10" s="65" t="s"/>
@@ -1363,7 +1244,7 @@
       <x:c r="I10" s="65" t="s"/>
       <x:c r="J10" s="65" t="s"/>
     </x:row>
-    <x:row r="11" spans="1:10" customFormat="1" ht="22.5" customHeight="1">
+    <x:row r="11" spans="1:11" customFormat="1" ht="22.5" customHeight="1">
       <x:c r="A11" s="45" t="s"/>
       <x:c r="B11" s="66" t="s">
         <x:v>12</x:v>
@@ -1393,7 +1274,7 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:10">
+    <x:row r="12" spans="1:11">
       <x:c r="A12" s="45" t="s"/>
       <x:c r="B12" s="68" t="n">
         <x:v>1023</x:v>
@@ -1419,7 +1300,7 @@
         <x:v>4674</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="13" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A13" s="45" t="s"/>
       <x:c r="B13" s="68" t="n">
         <x:v>1076</x:v>
@@ -1445,7 +1326,7 @@
         <x:v>17781</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="14" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A14" s="45" t="s"/>
       <x:c r="B14" s="68" t="n">
         <x:v>1123</x:v>
@@ -1471,7 +1352,7 @@
         <x:v>13945</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:10">
+    <x:row r="15" spans="1:11">
       <x:c r="A15" s="45" t="s"/>
       <x:c r="B15" s="68" t="n">
         <x:v>1169</x:v>
@@ -1497,7 +1378,7 @@
         <x:v>9471.95</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:10" customFormat="1" ht="12" customHeight="1">
+    <x:row r="16" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A16" s="45" t="s"/>
       <x:c r="B16" s="68" t="n">
         <x:v>1176</x:v>
@@ -1523,7 +1404,7 @@
         <x:v>4178.85</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:10">
+    <x:row r="17" spans="1:11">
       <x:c r="A17" s="45" t="s"/>
       <x:c r="B17" s="68" t="n">
         <x:v>1269</x:v>
@@ -1549,7 +1430,7 @@
         <x:v>1400</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:10">
+    <x:row r="18" spans="1:11">
       <x:c r="A18" s="45" t="s"/>
       <x:c r="B18" s="76" t="s"/>
       <x:c r="C18" s="76" t="s"/>
@@ -1565,7 +1446,7 @@
         <x:f>Subtotal(9,J12:J17)</x:f>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:10">
+    <x:row r="19" spans="1:11">
       <x:c r="A19" s="45" t="s"/>
       <x:c r="B19" s="65" t="s"/>
       <x:c r="C19" s="65" t="s"/>
@@ -1577,7 +1458,7 @@
       <x:c r="I19" s="75" t="s"/>
       <x:c r="J19" s="74" t="s"/>
     </x:row>
-    <x:row r="20" spans="1:10">
+    <x:row r="20" spans="1:11">
       <x:c r="A20" s="45" t="s"/>
       <x:c r="B20" s="50" t="s">
         <x:v>25</x:v>
@@ -1586,7 +1467,7 @@
         <x:v>26</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:10">
+    <x:row r="21" spans="1:11">
       <x:c r="A21" s="45" t="s"/>
       <x:c r="B21" s="73" t="s">
         <x:v>27</x:v>
@@ -1602,7 +1483,7 @@
   </x:sheetData>
   <x:phoneticPr fontId="0" type="noConversion"/>
   <x:conditionalFormatting sqref="E12:G17">
-    <x:cfRule type="expression" dxfId="2" priority="1" operator="equal">
+    <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <x:formula>$G12="Visa"</x:formula>
     </x:cfRule>
   </x:conditionalFormatting>
@@ -1613,4 +1494,199 @@
   <x:drawing r:id="rId2"/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:J7"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:10">
+      <x:c r="A1" s="45" t="s"/>
+      <x:c r="B1" s="68" t="n">
+        <x:v>1023</x:v>
+      </x:c>
+      <x:c r="C1" s="69">
+        <x:v>32325</x:v>
+      </x:c>
+      <x:c r="D1" s="69">
+        <x:v>32326</x:v>
+      </x:c>
+      <x:c r="E1" s="70" t="s"/>
+      <x:c r="F1" s="70" t="s"/>
+      <x:c r="G1" s="70" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="H1" s="71" t="n">
+        <x:v>4674</x:v>
+      </x:c>
+      <x:c r="I1" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J1" s="71" t="n">
+        <x:v>4674</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:10">
+      <x:c r="A2" s="45" t="s"/>
+      <x:c r="B2" s="68" t="n">
+        <x:v>1076</x:v>
+      </x:c>
+      <x:c r="C2" s="69">
+        <x:v>34684</x:v>
+      </x:c>
+      <x:c r="D2" s="69">
+        <x:v>32624</x:v>
+      </x:c>
+      <x:c r="E2" s="70" t="s"/>
+      <x:c r="F2" s="70" t="s"/>
+      <x:c r="G2" s="70" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H2" s="71" t="n">
+        <x:v>17781</x:v>
+      </x:c>
+      <x:c r="I2" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J2" s="71" t="n">
+        <x:v>17781</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:10">
+      <x:c r="A3" s="45" t="s"/>
+      <x:c r="B3" s="68" t="n">
+        <x:v>1123</x:v>
+      </x:c>
+      <x:c r="C3" s="69">
+        <x:v>34205</x:v>
+      </x:c>
+      <x:c r="D3" s="69">
+        <x:v>34205</x:v>
+      </x:c>
+      <x:c r="E3" s="70" t="s"/>
+      <x:c r="F3" s="70" t="s"/>
+      <x:c r="G3" s="70" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="H3" s="71" t="n">
+        <x:v>13945</x:v>
+      </x:c>
+      <x:c r="I3" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J3" s="71" t="n">
+        <x:v>13945</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:10">
+      <x:c r="A4" s="45" t="s"/>
+      <x:c r="B4" s="68" t="n">
+        <x:v>1169</x:v>
+      </x:c>
+      <x:c r="C4" s="69">
+        <x:v>34521</x:v>
+      </x:c>
+      <x:c r="D4" s="69">
+        <x:v>34521</x:v>
+      </x:c>
+      <x:c r="E4" s="70" t="s"/>
+      <x:c r="F4" s="70" t="s"/>
+      <x:c r="G4" s="70" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H4" s="71" t="n">
+        <x:v>9471.95</x:v>
+      </x:c>
+      <x:c r="I4" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J4" s="71" t="n">
+        <x:v>9471.95</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:10">
+      <x:c r="A5" s="45" t="s"/>
+      <x:c r="B5" s="68" t="n">
+        <x:v>1176</x:v>
+      </x:c>
+      <x:c r="C5" s="69">
+        <x:v>34541</x:v>
+      </x:c>
+      <x:c r="D5" s="69">
+        <x:v>34541</x:v>
+      </x:c>
+      <x:c r="E5" s="70" t="s"/>
+      <x:c r="F5" s="70" t="s"/>
+      <x:c r="G5" s="70" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H5" s="71" t="n">
+        <x:v>4178.85</x:v>
+      </x:c>
+      <x:c r="I5" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J5" s="71" t="n">
+        <x:v>4178.85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:10">
+      <x:c r="A6" s="45" t="s"/>
+      <x:c r="B6" s="68" t="n">
+        <x:v>1269</x:v>
+      </x:c>
+      <x:c r="C6" s="69">
+        <x:v>34684</x:v>
+      </x:c>
+      <x:c r="D6" s="69">
+        <x:v>34684</x:v>
+      </x:c>
+      <x:c r="E6" s="70" t="s"/>
+      <x:c r="F6" s="70" t="s"/>
+      <x:c r="G6" s="70" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H6" s="71" t="n">
+        <x:v>1400</x:v>
+      </x:c>
+      <x:c r="I6" s="71" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J6" s="71" t="n">
+        <x:v>1400</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:10">
+      <x:c r="A7" s="45" t="s"/>
+      <x:c r="B7" s="76" t="s"/>
+      <x:c r="C7" s="76" t="s"/>
+      <x:c r="D7" s="76" t="s"/>
+      <x:c r="E7" s="76" t="s"/>
+      <x:c r="F7" s="76" t="s"/>
+      <x:c r="G7" s="76" t="s"/>
+      <x:c r="H7" s="76" t="s"/>
+      <x:c r="I7" s="76" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J7" s="74" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:conditionalFormatting sqref="E1:G6">
+    <x:cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <x:formula>$G1="Visa"</x:formula>
+    </x:cfRule>
+  </x:conditionalFormatting>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>